<commit_message>
Work in PROGRESS - will tidy and comment as I go
</commit_message>
<xml_diff>
--- a/P1_TasksAndLinks.xlsx
+++ b/P1_TasksAndLinks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annmcnamara/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annmcnamara/National_Park_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBFE7624-2132-4F47-92DD-72DAD21BD994}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{289DBA95-83FF-F948-96BB-E84BEF27E01E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5500" yWindow="1780" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{59248C9D-8AFB-3C44-953A-2A0D00952DD0}"/>
+    <workbookView xWindow="5500" yWindow="1780" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{59248C9D-8AFB-3C44-953A-2A0D00952DD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
   <si>
     <t>Use Pandas to clean and format your dataset(s).</t>
   </si>
@@ -286,6 +286,15 @@
   </si>
   <si>
     <t>https://www.ducksters.com/geography/us_states/us_geographical_regions.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">It seems clear that unique keys to merge on are always </t>
+  </si>
+  <si>
+    <t>STATE ABBREVIATION</t>
+  </si>
+  <si>
+    <t>PARK CODE</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4E00D28-C0DA-464B-913E-D44DB04B60D1}">
   <dimension ref="A1:A33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -1380,12 +1389,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2858AD02-B537-E84B-A1F4-21FCE7BAA93C}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>